<commit_message>
transaccion inscripcion de producto
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/InscripcionProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/InscripcionProductos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>numero</t>
+  </si>
+  <si>
+    <t>tipoDocumentoInscripcion</t>
+  </si>
+  <si>
+    <t>numeroDocumentoInscripcion</t>
   </si>
   <si>
     <t>1</t>
@@ -133,9 +139,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -168,9 +174,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -192,6 +197,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -200,12 +206,57 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -217,6 +268,28 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,73 +309,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -325,49 +331,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,120 +512,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,21 +540,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -560,9 +551,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,21 +585,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -612,35 +599,54 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -656,124 +662,124 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1142,7 +1148,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1208,60 +1214,60 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2">
         <v>20580133845</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="2">
         <v>1044512658</v>
@@ -1269,40 +1275,40 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="7"/>
@@ -1312,40 +1318,40 @@
     </row>
     <row r="4" ht="15.75" spans="1:17">
       <c r="A4" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="H4" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>

</xml_diff>

<commit_message>
cambio de mapeo para inscripcion de productos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/InscripcionProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/InscripcionProductos.xlsx
@@ -103,7 +103,7 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>BANCOLOMBIA</t>
+    <t>Bancolombia</t>
   </si>
   <si>
     <t>Ahorros</t>
@@ -138,10 +138,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -175,7 +175,51 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,84 +241,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,25 +287,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -331,6 +331,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -343,19 +373,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,13 +481,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,133 +505,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,22 +540,50 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,45 +613,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -637,16 +626,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -662,124 +662,124 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>